<commit_message>
Updated to add 2024 handling and 2025 stocking data for Yuma Cove Backwater
</commit_message>
<xml_diff>
--- a/data/2024FallHarvest.xlsx
+++ b/data/2024FallHarvest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\YumaCoveBackwater\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5B0E8E-D5A5-47DB-9532-2336C17892DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F56612B-2269-45C1-AF13-83B38FCD4E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E8FAE24B-AFF9-44D0-A3FB-CAE30B48E00D}"/>
   </bookViews>
@@ -2326,7 +2326,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -2366,7 +2366,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2703,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50964F5-86B2-4683-8857-8ABD8A0F7045}">
   <dimension ref="A1:O368"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5125,7 +5125,7 @@
         <v>273</v>
       </c>
       <c r="G55">
-        <v>1160</v>
+        <v>160</v>
       </c>
       <c r="I55" t="s">
         <v>66</v>

</xml_diff>